<commit_message>
resolved exceed leave balance validation issue
</commit_message>
<xml_diff>
--- a/TestLogs.xlsx
+++ b/TestLogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\init-kopico\Library\java-spring-workspace\LeaveAppSystem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BDE3271-487C-4026-950D-0713BBE87D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BBD1B00-86FE-4ABE-9447-F670B8A1CF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0804F521-85FC-4DAD-A349-18373EB8A67E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Description</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Handling Teammate</t>
-  </si>
-  <si>
-    <t>Sunny</t>
   </si>
   <si>
     <t>Checking</t>
@@ -443,7 +440,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -485,9 +482,6 @@
     </row>
     <row r="2" spans="1:9">
       <c r="G2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>